<commit_message>
Cleaned sales and lead time data and merged into one df
</commit_message>
<xml_diff>
--- a/Beverage Costing.xlsx
+++ b/Beverage Costing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaspenney/Documents/McGill/MGSC 662/Skyline Group Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaspenney/Documents/McGill/MGSC 662/Skyline Group Project/MGSC-662-Skyline-Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D858C087-269F-A14C-BFE5-81AC94B9E6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5073011-4CA8-4843-A320-DB90AA1DC777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29400" yWindow="3220" windowWidth="29400" windowHeight="18380" xr2:uid="{741425EB-6119-46A9-84C2-B30F927C2C54}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{741425EB-6119-46A9-84C2-B30F927C2C54}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Menu" sheetId="4" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>Moscato White Dots, Australia</t>
   </si>
   <si>
-    <t>Rosé</t>
-  </si>
-  <si>
     <t>Chateau d'Esclands Whispering Angel, Côtes de Provence</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>Bright Eyes White Pinot, Central Otago</t>
-  </si>
-  <si>
-    <t>Terra Sancta Rosé, Central Otago</t>
   </si>
   <si>
     <t>Dessert Wine</t>
@@ -335,6 +329,12 @@
   </si>
   <si>
     <t>Stratosfare Moon Block, Central Otago</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Terra Sancta, Central Otago</t>
   </si>
 </sst>
 </file>
@@ -828,9 +828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BA09A1-1142-474B-9B10-13DFBA2A4DF8}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,22 +846,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -928,7 +928,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="14">
         <v>23</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="B17" s="12">
         <v>150</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="14">
         <v>19</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="14">
         <v>18</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B22" s="15">
         <v>17.5</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="12">
         <v>150</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="14">
         <v>14</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="14">
         <v>18</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="14">
         <v>18</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="14">
         <v>17</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B53" s="14">
         <v>17</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B66" s="14">
         <v>23</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B67" s="14">
         <v>22</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B68" s="14">
         <v>21</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B69" s="14">
         <v>20</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B70" s="14">
         <v>19</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B71" s="14">
         <v>18</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B76" s="14">
         <v>18</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B78" s="12">
         <v>150</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B81" s="14">
         <v>15</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -2672,6 +2672,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0b16c218-ad2c-4fc0-966d-45bbc55959f1" xsi:nil="true"/>
+    <Notes xmlns="a61e1c2a-19fc-4034-af01-4c7e82e894de" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a61e1c2a-19fc-4034-af01-4c7e82e894de">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035A26EEC667BCA4A8D4FADAB420D305F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41c30f238947c98a32a0afae7fb3a433">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a61e1c2a-19fc-4034-af01-4c7e82e894de" xmlns:ns3="0b16c218-ad2c-4fc0-966d-45bbc55959f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64bfffb5184bb8841afb570b7f19600f" ns2:_="" ns3:_="">
     <xsd:import namespace="a61e1c2a-19fc-4034-af01-4c7e82e894de"/>
@@ -2934,28 +2955,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0b16c218-ad2c-4fc0-966d-45bbc55959f1" xsi:nil="true"/>
-    <Notes xmlns="a61e1c2a-19fc-4034-af01-4c7e82e894de" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a61e1c2a-19fc-4034-af01-4c7e82e894de">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68899AE3-8498-4D70-B9A5-76737A7062C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0b16c218-ad2c-4fc0-966d-45bbc55959f1"/>
+    <ds:schemaRef ds:uri="a61e1c2a-19fc-4034-af01-4c7e82e894de"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8C17F26-079F-4735-88AB-71DC3FD4F468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B354EF3-DE79-4118-96DD-877A21B54768}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2972,29 +2997,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68899AE3-8498-4D70-B9A5-76737A7062C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0b16c218-ad2c-4fc0-966d-45bbc55959f1"/>
-    <ds:schemaRef ds:uri="a61e1c2a-19fc-4034-af01-4c7e82e894de"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8C17F26-079F-4735-88AB-71DC3FD4F468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>